<commit_message>
order extensibility and receipt ui
</commit_message>
<xml_diff>
--- a/data/menu_list.xlsx
+++ b/data/menu_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="79">
   <si>
     <t>name</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>3.8</t>
+  </si>
+  <si>
+    <t>04e97c9d-4c19-4a1a-9046-b975f194ac6a</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>fresh burger</t>
   </si>
 </sst>
 </file>
@@ -873,8 +882,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
menuitem and staff account update system
</commit_message>
<xml_diff>
--- a/data/menu_list.xlsx
+++ b/data/menu_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>fresh burger</t>
+  </si>
+  <si>
+    <t>Cole slaw</t>
   </si>
 </sst>
 </file>
@@ -710,7 +713,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -727,7 +730,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>

</xml_diff>